<commit_message>
AIP-1382 AIP-1322 Test Data Files for cabling with ph B &C
</commit_message>
<xml_diff>
--- a/AutoFirmwareUpgrade/CashelFirmwareAutomatedTest/TestDataFiles/FR_DISPATCHRMS_DATASET_18Channel/1U3I_PhaseB.xlsx
+++ b/AutoFirmwareUpgrade/CashelFirmwareAutomatedTest/TestDataFiles/FR_DISPATCHRMS_DATASET_18Channel/1U3I_PhaseB.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E0CA81-3588-42E4-B040-987ACD8D4A8D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A56780-F5C6-454A-AE14-AA1701EFBB24}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StandaloneParameters" sheetId="6" r:id="rId1"/>
@@ -13804,7 +13804,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13833,7 +13833,7 @@
         <v>84</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -13953,7 +13953,7 @@
         <v>99</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -14151,7 +14151,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14195,13 +14195,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -14265,7 +14265,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>6</v>

</xml_diff>